<commit_message>
planilha criada no doc, só falta passar para o doc inicial
</commit_message>
<xml_diff>
--- a/pandas_to_excel.xlsx
+++ b/pandas_to_excel.xlsx
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -132,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -142,10 +145,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,88 +523,108 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.7109375" customWidth="1" min="1" max="1"/>
-    <col width="40.7109375" customWidth="1" min="2" max="2"/>
-    <col width="3.7109375" customWidth="1" min="3" max="3"/>
-    <col width="13.7109375" customWidth="1" min="4" max="4"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>VOITHPAPESPPROLIANT</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n"/>
-      <c r="C2" s="3" t="n"/>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
       <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
+      <c r="F2" s="5" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>HPE Tech Care Basic SVC</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
+      <c r="B3" s="4" t="n"/>
+      <c r="C3" s="4" t="n"/>
       <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Vigência - De:</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>45778</v>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Vigência - Até:</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>46142</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>Part Number</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Hardware</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C5" s="8" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>Serial Number</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>HU4A2AC</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>HPE Hardware Tech Support</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>1</v>
+      <c r="E5" s="8" t="inlineStr">
+        <is>
+          <t>Net Price</t>
+        </is>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>Net Value</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>863442-B21</t>
+          <t>HU4A2AC</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>HPE BL460c Gen10 10Gb/20Gb FLB CTO Blade</t>
+          <t>HPE Hardware Tech Support</t>
         </is>
       </c>
       <c r="C6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>BRC841B4PF</t>
-        </is>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -619,8 +643,14 @@
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PG</t>
-        </is>
+          <t>BRC841B4PF</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>226.15</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>2713.8</v>
       </c>
     </row>
     <row r="8">
@@ -639,8 +669,14 @@
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PK</t>
-        </is>
+          <t>BRC841B4PG</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>226.15</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>2713.8</v>
       </c>
     </row>
     <row r="9">
@@ -659,8 +695,14 @@
       </c>
       <c r="D9" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PJ</t>
-        </is>
+          <t>BRC841B4PK</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>226.15</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>2713.8</v>
       </c>
     </row>
     <row r="10">
@@ -679,43 +721,61 @@
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PH</t>
-        </is>
+          <t>BRC841B4PJ</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>226.15</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>2713.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>HU4A1AC</t>
+          <t>863442-B21</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>HPE Remote Tech Support</t>
+          <t>HPE BL460c Gen10 10Gb/20Gb FLB CTO Blade</t>
         </is>
       </c>
       <c r="C11" s="6" t="n">
         <v>1</v>
+      </c>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>BRC841B4PH</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>226.15</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>2713.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>863442-B21</t>
+          <t>HU4A1AC</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>HPE BL460c Gen10 10Gb/20Gb FLB CTO Blade</t>
+          <t>HPE Remote Tech Support</t>
         </is>
       </c>
       <c r="C12" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="6" t="inlineStr">
-        <is>
-          <t>BRC841B4PF</t>
-        </is>
+      <c r="E12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -734,8 +794,14 @@
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PG</t>
-        </is>
+          <t>BRC841B4PF</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>36.27</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>435.24</v>
       </c>
     </row>
     <row r="14">
@@ -754,8 +820,14 @@
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PK</t>
-        </is>
+          <t>BRC841B4PG</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>36.27</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>435.24</v>
       </c>
     </row>
     <row r="15">
@@ -774,8 +846,14 @@
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
-          <t>BRC841B4PJ</t>
-        </is>
+          <t>BRC841B4PK</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>36.27</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>435.24</v>
       </c>
     </row>
     <row r="16">
@@ -794,102 +872,137 @@
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
+          <t>BRC841B4PJ</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>36.27</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>435.24</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>863442-B21</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c Gen10 10Gb/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
           <t>BRC841B4PH</t>
         </is>
       </c>
-    </row>
-    <row r="17"/>
+      <c r="E17" s="6" t="n">
+        <v>36.27</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>435.24</v>
+      </c>
+    </row>
     <row r="18"/>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
         <is>
           <t>VOITHPAPSP-PROLIANTC</t>
         </is>
       </c>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="3" t="n"/>
-      <c r="D19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="B20" s="4" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="4" t="n"/>
+      <c r="E20" s="4" t="n"/>
+      <c r="F20" s="5" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>HPE Tech Care Basic SVC</t>
         </is>
       </c>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="B21" s="5" t="inlineStr">
-        <is>
-          <t>Hardware</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="inlineStr">
-        <is>
-          <t>Qty</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="inlineStr">
-        <is>
-          <t>Serial Number</t>
-        </is>
-      </c>
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="4" t="n"/>
+      <c r="E21" s="4" t="n"/>
+      <c r="F21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>HU4A2AC</t>
-        </is>
-      </c>
-      <c r="B22" s="6" t="inlineStr">
-        <is>
-          <t>HPE Hardware Tech Support</t>
-        </is>
-      </c>
-      <c r="C22" s="6" t="n">
-        <v>1</v>
+          <t>Vigência - De:</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>45778</v>
+      </c>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>Vigência - Até:</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>46142</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="inlineStr">
-        <is>
-          <t>755258-B21</t>
-        </is>
-      </c>
-      <c r="B23" s="6" t="inlineStr">
-        <is>
-          <t>HPE DL360 Gen9 8SFF CTO Server</t>
-        </is>
-      </c>
-      <c r="C23" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6" t="inlineStr">
-        <is>
-          <t>BRC551773B</t>
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>Hardware</t>
+        </is>
+      </c>
+      <c r="C23" s="8" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>Net Price</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>Net Value</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>HU4A1AC</t>
+          <t>HU4A2AC</t>
         </is>
       </c>
       <c r="B24" s="6" t="inlineStr">
         <is>
-          <t>HPE Remote Tech Support</t>
+          <t>HPE Hardware Tech Support</t>
         </is>
       </c>
       <c r="C24" s="6" t="n">
         <v>1</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -911,198 +1024,183 @@
           <t>BRC551773B</t>
         </is>
       </c>
-    </row>
-    <row r="26"/>
+      <c r="E25" s="6" t="n">
+        <v>394.72</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <v>4736.64</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>HU4A1AC</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>HPE Remote Tech Support</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>755258-B21</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>HPE DL360 Gen9 8SFF CTO Server</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="inlineStr">
+        <is>
+          <t>BRC551773B</t>
+        </is>
+      </c>
+      <c r="E27" s="6" t="n">
+        <v>80.94</v>
+      </c>
+      <c r="F27" s="6" t="n">
+        <v>971.28</v>
+      </c>
+    </row>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32">
+      <c r="A32" s="3" t="inlineStr">
         <is>
           <t>VOITHPAPSP-PROLIANT</t>
         </is>
       </c>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="3" t="n"/>
-      <c r="D27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
+      <c r="B32" s="4" t="n"/>
+      <c r="C32" s="4" t="n"/>
+      <c r="D32" s="4" t="n"/>
+      <c r="E32" s="4" t="n"/>
+      <c r="F32" s="5" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>HPE Tech Care Basic SVC</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n"/>
-      <c r="C28" s="3" t="n"/>
-      <c r="D28" s="4" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="B29" s="5" t="inlineStr">
-        <is>
-          <t>Hardware</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="inlineStr">
-        <is>
-          <t>Qty</t>
-        </is>
-      </c>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>Serial Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="inlineStr">
-        <is>
-          <t>HU4A2AC</t>
-        </is>
-      </c>
-      <c r="B30" s="6" t="inlineStr">
-        <is>
-          <t>HPE Hardware Tech Support</t>
-        </is>
-      </c>
-      <c r="C30" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="inlineStr">
-        <is>
-          <t>813198-B21</t>
-        </is>
-      </c>
-      <c r="B31" s="6" t="inlineStr">
-        <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
-        </is>
-      </c>
-      <c r="C31" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6" t="inlineStr">
-        <is>
-          <t>BRC7419854</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="6" t="inlineStr">
-        <is>
-          <t>813198-B21</t>
-        </is>
-      </c>
-      <c r="B32" s="6" t="inlineStr">
-        <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
-        </is>
-      </c>
-      <c r="C32" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6" t="inlineStr">
-        <is>
-          <t>BRC7419855</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="6" t="inlineStr">
-        <is>
-          <t>813198-B21</t>
-        </is>
-      </c>
-      <c r="B33" s="6" t="inlineStr">
-        <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
-        </is>
-      </c>
-      <c r="C33" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6" t="inlineStr">
-        <is>
-          <t>BRC7419853</t>
-        </is>
-      </c>
+      <c r="B33" s="4" t="n"/>
+      <c r="C33" s="4" t="n"/>
+      <c r="D33" s="4" t="n"/>
+      <c r="E33" s="4" t="n"/>
+      <c r="F33" s="5" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>813198-B21</t>
-        </is>
-      </c>
-      <c r="B34" s="6" t="inlineStr">
-        <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
-        </is>
-      </c>
-      <c r="C34" s="6" t="n">
-        <v>1</v>
+          <t>Vigência - De:</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>45778</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>BRC7419851</t>
-        </is>
+          <t>Vigência - Até:</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="n">
+        <v>46142</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="inlineStr">
-        <is>
-          <t>813198-B21</t>
-        </is>
-      </c>
-      <c r="B35" s="6" t="inlineStr">
-        <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
-        </is>
-      </c>
-      <c r="C35" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6" t="inlineStr">
-        <is>
-          <t>BRC7419852</t>
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>Hardware</t>
+        </is>
+      </c>
+      <c r="C35" s="8" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="D35" s="8" t="inlineStr">
+        <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+      <c r="E35" s="8" t="inlineStr">
+        <is>
+          <t>Net Price</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="inlineStr">
+        <is>
+          <t>Net Value</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>813198-B21</t>
+          <t>HU4A2AC</t>
         </is>
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+          <t>HPE Hardware Tech Support</t>
         </is>
       </c>
       <c r="C36" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="6" t="inlineStr">
-        <is>
-          <t>BRC7419856</t>
-        </is>
+      <c r="E36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>HU4A1AC</t>
+          <t>813198-B21</t>
         </is>
       </c>
       <c r="B37" s="6" t="inlineStr">
         <is>
-          <t>HPE Remote Tech Support</t>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
         </is>
       </c>
       <c r="C37" s="6" t="n">
         <v>1</v>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419854</t>
+        </is>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="38">
@@ -1121,8 +1219,14 @@
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
-          <t>BRC7419854</t>
-        </is>
+          <t>BRC7419855</t>
+        </is>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F38" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="39">
@@ -1141,8 +1245,14 @@
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
-          <t>BRC7419855</t>
-        </is>
+          <t>BRC7419853</t>
+        </is>
+      </c>
+      <c r="E39" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F39" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="40">
@@ -1161,8 +1271,14 @@
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>BRC7419853</t>
-        </is>
+          <t>BRC7419851</t>
+        </is>
+      </c>
+      <c r="E40" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F40" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="41">
@@ -1181,8 +1297,14 @@
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
-          <t>BRC7419851</t>
-        </is>
+          <t>BRC7419852</t>
+        </is>
+      </c>
+      <c r="E41" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F41" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="42">
@@ -1201,38 +1323,201 @@
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>BRC7419852</t>
-        </is>
+          <t>BRC7419856</t>
+        </is>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>322.95</v>
+      </c>
+      <c r="F42" s="6" t="n">
+        <v>3875.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
         <is>
+          <t>HU4A1AC</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>HPE Remote Tech Support</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="inlineStr">
+        <is>
           <t>813198-B21</t>
         </is>
       </c>
-      <c r="B43" s="6" t="inlineStr">
+      <c r="B44" s="6" t="inlineStr">
         <is>
           <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
         </is>
       </c>
-      <c r="C43" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="6" t="inlineStr">
+      <c r="C44" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419854</t>
+        </is>
+      </c>
+      <c r="E44" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F44" s="6" t="n">
+        <v>453.24</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>813198-B21</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419855</t>
+        </is>
+      </c>
+      <c r="E45" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F45" s="6" t="n">
+        <v>453.24</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="inlineStr">
+        <is>
+          <t>813198-B21</t>
+        </is>
+      </c>
+      <c r="B46" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C46" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419853</t>
+        </is>
+      </c>
+      <c r="E46" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>453.24</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>813198-B21</t>
+        </is>
+      </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C47" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419851</t>
+        </is>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>453.24</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>813198-B21</t>
+        </is>
+      </c>
+      <c r="B48" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C48" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>BRC7419852</t>
+        </is>
+      </c>
+      <c r="E48" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F48" s="6" t="n">
+        <v>453.24</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>813198-B21</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>HPE BL460c G9 E5v4 10/20Gb FLB CTO Blade</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
         <is>
           <t>BRC7419856</t>
         </is>
+      </c>
+      <c r="E49" s="6" t="n">
+        <v>37.77</v>
+      </c>
+      <c r="F49" s="6" t="n">
+        <v>453.24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>